<commit_message>
Fix css class name and add test files.
</commit_message>
<xml_diff>
--- a/tests/order-variable-settings/additional_platform.xlsx
+++ b/tests/order-variable-settings/additional_platform.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="94">
   <si>
     <t>받는분성명</t>
   </si>
@@ -65,10 +65,10 @@
     <t>{order_id}</t>
   </si>
   <si>
-    <t>Platform Name</t>
-  </si>
-  <si>
-    <t>Header Row</t>
+    <t>PlatformName</t>
+  </si>
+  <si>
+    <t>HeaderRow</t>
   </si>
   <si>
     <t>order_id</t>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>ADDITIONALADDRESS</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>PHONE</t>
@@ -307,7 +304,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +315,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -384,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,13 +419,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -737,7 +737,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="7" width="17.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="7" width="23.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
@@ -831,274 +831,272 @@
       <c r="J2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="O2" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="O4" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="10">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="10">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>